<commit_message>
añaden excel con todas las mallas, se sacand datos desde un excel
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\practica2\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A0041F-4D60-4E8A-8B4F-A7B612A55EF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8790182B-2EB1-4CF0-89C5-BEEF8C37ECA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,7 +2635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A12D3C-F185-4C2F-BC8E-E636E865D27E}">
   <dimension ref="A2:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improve asigation of weight
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF7497-06A2-4B6D-B25C-8A137D5E0AB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB337D42-C32B-4874-8C4D-B8D4565C6BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="4545" yWindow="1290" windowWidth="18000" windowHeight="9810" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>MODELOS ESTOCASTICOS Y SIMULACIÓN</t>
   </si>
   <si>
-    <t>GESTIÓN ORGANIZACIÓNAL</t>
-  </si>
-  <si>
     <t>EVALUACIÓN DE PROYECTOS TIC</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>GESTIÓN ORGANIZACIONAL</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1157,7 +1157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1455,11 +1455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1487,10 +1487,10 @@
         <v>52</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="21">
         <v>1</v>
@@ -1546,7 +1546,7 @@
         <v>76</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" s="21">
         <v>1</v>
@@ -1585,7 +1585,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1651,7 +1651,7 @@
         <v>66</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="22">
         <v>2</v>
@@ -1693,7 +1693,7 @@
         <v>65</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" s="22">
         <v>2</v>
@@ -1720,7 +1720,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="23"/>
     </row>
@@ -1756,13 +1756,13 @@
         <v>67</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G15" s="23"/>
     </row>
@@ -1786,7 +1786,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>60</v>
@@ -1829,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="24"/>
     </row>
@@ -1844,16 +1844,16 @@
         <v>75</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="24">
         <v>4</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" s="24"/>
     </row>
@@ -1897,7 +1897,7 @@
         <v>14</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>65</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="24">
         <v>4</v>
@@ -1929,7 +1929,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1959,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" s="25"/>
     </row>
@@ -1971,7 +1971,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>62</v>
@@ -1983,7 +1983,7 @@
         <v>18</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2003,10 +2003,10 @@
         <v>5</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>83</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="25">
         <v>5</v>
@@ -2029,7 +2029,7 @@
         <v>19</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2043,7 +2043,7 @@
         <v>65</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E28" s="25">
         <v>5</v>
@@ -2061,10 +2061,10 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E29" s="25">
         <v>5</v>
@@ -2073,7 +2073,7 @@
         <v>21</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J29" s="31"/>
     </row>
@@ -2085,10 +2085,10 @@
         <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" s="26">
         <v>6</v>
@@ -2097,7 +2097,7 @@
         <v>12</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2111,16 +2111,16 @@
         <v>95</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E31" s="26">
         <v>6</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2140,10 +2140,10 @@
         <v>6</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2163,10 +2163,10 @@
         <v>6</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>23</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>61</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2256,7 +2256,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2267,10 +2267,10 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E38" s="27">
         <v>7</v>
@@ -2291,7 +2291,7 @@
         <v>91</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" s="27">
         <v>7</v>
@@ -2300,7 +2300,7 @@
         <v>32</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2311,10 +2311,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>96</v>
+        <v>290</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E40" s="28">
         <v>8</v>
@@ -2323,7 +2323,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>85</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E41" s="28">
         <v>8</v>
@@ -2346,7 +2346,7 @@
         <v>34</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2360,7 +2360,7 @@
         <v>92</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
@@ -2369,7 +2369,7 @@
         <v>31</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2389,10 +2389,10 @@
         <v>8</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>65</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E44" s="28">
         <v>8</v>
@@ -2427,7 +2427,7 @@
         <v>38</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" s="29">
         <v>9</v>
@@ -2448,7 +2448,7 @@
         <v>38</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="29">
         <v>9</v>
@@ -2469,7 +2469,7 @@
         <v>38</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E47" s="29">
         <v>9</v>
@@ -2487,7 +2487,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -2496,10 +2496,10 @@
         <v>9</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>38</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E49" s="29">
         <v>9</v>
@@ -2534,7 +2534,7 @@
         <v>38</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E50" s="30">
         <v>10</v>
@@ -2555,7 +2555,7 @@
         <v>38</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E51" s="30">
         <v>10</v>
@@ -2576,7 +2576,7 @@
         <v>38</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E52" s="30">
         <v>10</v>
@@ -2594,10 +2594,10 @@
         <v>47</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E53" s="30">
         <v>10</v>
@@ -2606,7 +2606,7 @@
         <v>46</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>38</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E54" s="30">
         <v>10</v>
@@ -2635,19 +2635,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E55" s="30">
         <v>11</v>
       </c>
       <c r="F55" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G55" s="30"/>
     </row>
@@ -2665,7 +2665,7 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
@@ -2676,22 +2676,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="C2" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>149</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2699,10 +2699,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>37</v>
@@ -2717,10 +2717,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>35</v>
@@ -2735,10 +2735,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>22</v>
@@ -2747,7 +2747,7 @@
         <v>54</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,10 +2755,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>30</v>
@@ -2773,10 +2773,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>37</v>
@@ -2791,10 +2791,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>30</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="38" t="s">
         <v>165</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>166</v>
       </c>
       <c r="E9" s="39">
         <v>54</v>
@@ -2827,19 +2827,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>169</v>
-      </c>
       <c r="E10" s="39">
         <v>54</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2847,13 +2847,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="D11" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E11" s="39">
         <v>54</v>
@@ -2865,19 +2865,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>174</v>
-      </c>
       <c r="E12" s="39">
         <v>54</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,13 +2885,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="38" t="s">
         <v>176</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>177</v>
       </c>
       <c r="E13" s="39">
         <v>54</v>
@@ -2903,13 +2903,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="38" t="s">
         <v>179</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>180</v>
       </c>
       <c r="E14" s="39">
         <v>54</v>
@@ -2921,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>22</v>
@@ -2939,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>37</v>
@@ -2957,10 +2957,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>37</v>
@@ -2975,10 +2975,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>22</v>
@@ -2993,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="39">
@@ -3009,13 +3009,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>193</v>
       </c>
       <c r="E20" s="39">
         <v>54</v>
@@ -3027,13 +3027,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>195</v>
-      </c>
       <c r="D21" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="39">
         <v>54</v>
@@ -3045,13 +3045,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="38" t="s">
         <v>197</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>198</v>
       </c>
       <c r="E22" s="39">
         <v>54</v>
@@ -3063,10 +3063,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>17</v>
@@ -3081,19 +3081,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="E24" s="39">
+        <v>54</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>203</v>
-      </c>
-      <c r="E24" s="39">
-        <v>54</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3101,13 +3101,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="38" t="s">
         <v>206</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>207</v>
       </c>
       <c r="E25" s="39">
         <v>54</v>
@@ -3119,13 +3119,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="38" t="s">
         <v>209</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>210</v>
       </c>
       <c r="E26" s="39">
         <v>54</v>
@@ -3137,10 +3137,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>37</v>
@@ -3155,13 +3155,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="38" t="s">
         <v>214</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>215</v>
       </c>
       <c r="E28" s="39">
         <v>54</v>
@@ -3173,13 +3173,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="38" t="s">
         <v>217</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>218</v>
       </c>
       <c r="E29" s="39">
         <v>54</v>
@@ -3191,10 +3191,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>30</v>
@@ -3209,10 +3209,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>22</v>
@@ -3227,13 +3227,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>224</v>
-      </c>
       <c r="D32" s="38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E32" s="39">
         <v>54</v>
@@ -3245,10 +3245,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>37</v>
@@ -3257,7 +3257,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3265,13 +3265,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="38" t="s">
         <v>229</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>230</v>
       </c>
       <c r="E34" s="39">
         <v>54</v>
@@ -3283,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>30</v>
@@ -3301,10 +3301,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>30</v>
@@ -3319,13 +3319,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="38" t="s">
         <v>236</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>237</v>
       </c>
       <c r="E37" s="39">
         <v>54</v>
@@ -3337,13 +3337,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="38" t="s">
         <v>239</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>240</v>
       </c>
       <c r="E38" s="39">
         <v>54</v>
@@ -3355,13 +3355,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="38" t="s">
         <v>242</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>243</v>
       </c>
       <c r="E39" s="39">
         <v>54</v>
@@ -3373,10 +3373,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>36</v>
@@ -3391,13 +3391,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="D41" s="38" t="s">
         <v>247</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>248</v>
       </c>
       <c r="E41" s="39">
         <v>54</v>
@@ -3409,10 +3409,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>31</v>
@@ -3427,10 +3427,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="D43" s="38" t="s">
         <v>37</v>
@@ -3445,10 +3445,10 @@
         <v>2</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="D44" s="38" t="s">
         <v>31</v>
@@ -3463,10 +3463,10 @@
         <v>2</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>36</v>
@@ -3481,13 +3481,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>258</v>
-      </c>
       <c r="D46" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E46" s="39">
         <v>54</v>
@@ -3499,13 +3499,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="D47" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E47" s="39">
         <v>54</v>
@@ -3517,10 +3517,10 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>31</v>
@@ -3535,13 +3535,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="38" t="s">
         <v>264</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>265</v>
       </c>
       <c r="E49" s="39">
         <v>54</v>
@@ -3553,13 +3553,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="38" t="s">
         <v>267</v>
-      </c>
-      <c r="D50" s="38" t="s">
-        <v>268</v>
       </c>
       <c r="E50" s="39">
         <v>54</v>
@@ -3571,10 +3571,10 @@
         <v>2</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>270</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>36</v>
@@ -3589,10 +3589,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>22</v>
@@ -3607,10 +3607,10 @@
         <v>2</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>33</v>
@@ -3625,10 +3625,10 @@
         <v>2</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>31</v>
@@ -3637,7 +3637,7 @@
         <v>54</v>
       </c>
       <c r="F54" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3645,13 +3645,13 @@
         <v>2</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="D55" s="38" t="s">
         <v>279</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>280</v>
       </c>
       <c r="E55" s="39">
         <v>54</v>
@@ -3667,11 +3667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218295B3-95C6-4056-8916-38091AF1344F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
@@ -3680,10 +3680,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>284</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3691,7 +3691,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3699,7 +3699,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3707,15 +3707,15 @@
         <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
         <v>95</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3731,7 +3731,7 @@
         <v>90</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3739,7 +3739,7 @@
         <v>91</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3747,7 +3747,7 @@
         <v>85</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3755,12 +3755,12 @@
         <v>94</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
pseudo algoritmo hecho para electivos. CFG será similar. Solucionar errores pronto
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB082E67-03B3-4975-8920-349EA60F2CF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F8651-4962-4509-8A0F-79E7936F6F77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="278">
   <si>
     <t>CBM1000</t>
   </si>
@@ -154,36 +154,12 @@
     <t>Electivo Profesional</t>
   </si>
   <si>
-    <t>CIT33XX-1</t>
-  </si>
-  <si>
-    <t>CIT34XX-1</t>
-  </si>
-  <si>
-    <t>CIT34XX-2</t>
-  </si>
-  <si>
     <t>CIT3200</t>
   </si>
   <si>
-    <t>CIT33XX-2</t>
-  </si>
-  <si>
-    <t>CIT33XX-3</t>
-  </si>
-  <si>
-    <t>CIT34XX-3</t>
-  </si>
-  <si>
-    <t>CIT34XX-4</t>
-  </si>
-  <si>
     <t>CIT3201</t>
   </si>
   <si>
-    <t>CIT33XX-4</t>
-  </si>
-  <si>
     <t>Código</t>
   </si>
   <si>
@@ -334,12 +310,6 @@
     <t>COMUNICACIÓN PARA LA INGENIERÍA</t>
   </si>
   <si>
-    <t>INGLÉS I</t>
-  </si>
-  <si>
-    <t>INGLÉS II</t>
-  </si>
-  <si>
     <t>DERECHO EN INGENIERÍA</t>
   </si>
   <si>
@@ -400,9 +370,6 @@
     <t>Prerreq</t>
   </si>
   <si>
-    <t>Equivalencias</t>
-  </si>
-  <si>
     <t>CIT2109</t>
   </si>
   <si>
@@ -431,9 +398,6 @@
   </si>
   <si>
     <t>CIT2012</t>
-  </si>
-  <si>
-    <t>CIG1012</t>
   </si>
   <si>
     <t>CII2100</t>
@@ -879,37 +843,34 @@
     <t>CIT2102, CIT2200</t>
   </si>
   <si>
-    <t>ESTRUCTURAS DE DATOS Y ALGORITMOS</t>
-  </si>
-  <si>
-    <t>DESARROLLO WEB Y MÓVIL</t>
+    <t>Malla 2010</t>
+  </si>
+  <si>
+    <t>Malla 2020</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>GESTIÓN ORGANIZACIONAL</t>
+  </si>
+  <si>
+    <t>CIG1002</t>
+  </si>
+  <si>
+    <t>CIG1003</t>
   </si>
   <si>
     <t>INGLÉS GENERAL I</t>
   </si>
   <si>
-    <t>Malla 2010</t>
-  </si>
-  <si>
-    <t>Malla 2020</t>
-  </si>
-  <si>
-    <t>TALLER DE REDES Y SERVICIOS</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA Y ORGANIZ DE COMPUTADORES</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA DE SOFTWARE</t>
-  </si>
-  <si>
-    <t>DATA SCIENCE</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>GESTIÓN ORGANIZACIONAL</t>
+    <t>INGLÉS GENERAL II</t>
+  </si>
+  <si>
+    <t>CIT33XX</t>
+  </si>
+  <si>
+    <t>CIT34XX</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1127,6 +1088,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1455,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,30 +1432,27 @@
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1501,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E3" s="21">
         <v>1</v>
@@ -1512,9 +1471,8 @@
       <c r="F3" s="12">
         <v>0</v>
       </c>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1522,10 +1480,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
@@ -1533,9 +1491,8 @@
       <c r="F4" s="12">
         <v>0</v>
       </c>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1543,10 +1500,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E5" s="21">
         <v>1</v>
@@ -1554,9 +1511,8 @@
       <c r="F5" s="12">
         <v>0</v>
       </c>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1564,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D6" s="12">
         <v>9</v>
@@ -1575,9 +1531,8 @@
       <c r="F6" s="12">
         <v>0</v>
       </c>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1585,7 +1540,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1596,9 +1551,8 @@
       <c r="F7" s="12">
         <v>0</v>
       </c>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1606,10 +1560,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E8" s="22">
         <v>2</v>
@@ -1617,9 +1571,8 @@
       <c r="F8" s="13">
         <v>1</v>
       </c>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1627,10 +1580,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E9" s="22">
         <v>2</v>
@@ -1638,9 +1591,8 @@
       <c r="F9" s="13">
         <v>2</v>
       </c>
-      <c r="G9" s="22"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1648,10 +1600,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E10" s="22">
         <v>2</v>
@@ -1659,9 +1611,8 @@
       <c r="F10" s="13">
         <v>2</v>
       </c>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1669,10 +1620,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E11" s="22">
         <v>2</v>
@@ -1680,20 +1631,19 @@
       <c r="F11" s="13">
         <v>4</v>
       </c>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E12" s="22">
         <v>2</v>
@@ -1701,9 +1651,8 @@
       <c r="F12" s="13">
         <v>0</v>
       </c>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1711,7 +1660,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D13" s="14">
         <v>18</v>
@@ -1720,11 +1669,10 @@
         <v>3</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1732,10 +1680,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E14" s="23">
         <v>3</v>
@@ -1743,9 +1691,8 @@
       <c r="F14" s="14">
         <v>7</v>
       </c>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1753,20 +1700,19 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E15" s="23">
         <v>3</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1774,7 +1720,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D16" s="14">
         <v>19</v>
@@ -1784,9 +1730,6 @@
       </c>
       <c r="F16" s="14">
         <v>9</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1797,19 +1740,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E17" s="23">
         <v>3</v>
       </c>
       <c r="F17" s="14">
         <v>9</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1820,18 +1760,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E18" s="24">
         <v>4</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="24"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1841,19 +1780,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E19" s="24">
         <v>4</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1864,7 +1800,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D20" s="15">
         <v>23</v>
@@ -1873,9 +1809,8 @@
         <v>4</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="24"/>
+        <v>105</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1885,19 +1820,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E21" s="24">
         <v>4</v>
       </c>
       <c r="F21" s="15">
         <v>14</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1905,13 +1837,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E22" s="24">
         <v>4</v>
@@ -1919,7 +1851,6 @@
       <c r="F22" s="15">
         <v>0</v>
       </c>
-      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1929,7 +1860,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>99</v>
+        <v>274</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1940,7 +1871,6 @@
       <c r="F23" s="15">
         <v>5</v>
       </c>
-      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -1950,7 +1880,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D24" s="16">
         <v>29</v>
@@ -1959,9 +1889,8 @@
         <v>5</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="25"/>
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1971,19 +1900,16 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E25" s="25">
         <v>5</v>
       </c>
       <c r="F25" s="33">
         <v>18</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1994,19 +1920,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E26" s="25">
         <v>5</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2017,19 +1940,16 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E27" s="25">
         <v>5</v>
       </c>
       <c r="F27" s="16">
         <v>19</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2037,13 +1957,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E28" s="25">
         <v>5</v>
@@ -2051,7 +1971,6 @@
       <c r="F28" s="16">
         <v>0</v>
       </c>
-      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -2061,19 +1980,16 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E29" s="25">
         <v>5</v>
       </c>
       <c r="F29" s="16">
         <v>21</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>132</v>
       </c>
       <c r="J29" s="31"/>
     </row>
@@ -2085,19 +2001,16 @@
         <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E30" s="26">
         <v>6</v>
       </c>
       <c r="F30" s="17">
         <v>12</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2108,19 +2021,16 @@
         <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E31" s="26">
         <v>6</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2131,7 +2041,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D32" s="17">
         <v>35</v>
@@ -2140,13 +2050,10 @@
         <v>6</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -2154,7 +2061,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D33" s="17">
         <v>40</v>
@@ -2163,13 +2070,10 @@
         <v>6</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -2177,7 +2081,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D34" s="17">
         <v>37</v>
@@ -2188,11 +2092,8 @@
       <c r="F34" s="17">
         <v>23</v>
       </c>
-      <c r="G34" s="26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>33</v>
       </c>
@@ -2200,7 +2101,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D35" s="18">
         <v>46</v>
@@ -2211,9 +2112,8 @@
       <c r="F35" s="18">
         <v>2</v>
       </c>
-      <c r="G35" s="27"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>34</v>
       </c>
@@ -2221,22 +2121,19 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E36" s="27">
         <v>7</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>35</v>
       </c>
@@ -2244,7 +2141,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D37" s="18">
         <v>41</v>
@@ -2255,11 +2152,8 @@
       <c r="F37" s="18">
         <v>30</v>
       </c>
-      <c r="G37" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>36</v>
       </c>
@@ -2267,10 +2161,10 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E38" s="27">
         <v>7</v>
@@ -2278,9 +2172,8 @@
       <c r="F38" s="18">
         <v>0</v>
       </c>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>37</v>
       </c>
@@ -2288,10 +2181,10 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E39" s="27">
         <v>7</v>
@@ -2299,11 +2192,8 @@
       <c r="F39" s="18">
         <v>32</v>
       </c>
-      <c r="G39" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
@@ -2311,10 +2201,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E40" s="28">
         <v>8</v>
@@ -2322,11 +2212,8 @@
       <c r="F40" s="19">
         <v>5</v>
       </c>
-      <c r="G40" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
@@ -2334,10 +2221,10 @@
         <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E41" s="28">
         <v>8</v>
@@ -2345,11 +2232,8 @@
       <c r="F41" s="19">
         <v>34</v>
       </c>
-      <c r="G41" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>40</v>
       </c>
@@ -2357,10 +2241,10 @@
         <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
@@ -2368,11 +2252,8 @@
       <c r="F42" s="19">
         <v>31</v>
       </c>
-      <c r="G42" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>41</v>
       </c>
@@ -2380,7 +2261,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D43" s="19">
         <v>46</v>
@@ -2389,24 +2270,21 @@
         <v>8</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="G43" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E44" s="28">
         <v>8</v>
@@ -2414,20 +2292,19 @@
       <c r="F44" s="19">
         <v>0</v>
       </c>
-      <c r="G44" s="28"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>39</v>
+        <v>276</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E45" s="29">
         <v>9</v>
@@ -2435,20 +2312,19 @@
       <c r="F45" s="20">
         <v>0</v>
       </c>
-      <c r="G45" s="29"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>40</v>
+        <v>277</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E46" s="29">
         <v>9</v>
@@ -2456,20 +2332,19 @@
       <c r="F46" s="20">
         <v>0</v>
       </c>
-      <c r="G46" s="29"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>41</v>
+        <v>277</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E47" s="29">
         <v>9</v>
@@ -2477,17 +2352,16 @@
       <c r="F47" s="20">
         <v>0</v>
       </c>
-      <c r="G47" s="29"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -2496,24 +2370,21 @@
         <v>9</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="G48" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>43</v>
+        <v>276</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E49" s="29">
         <v>9</v>
@@ -2521,20 +2392,19 @@
       <c r="F49" s="20">
         <v>0</v>
       </c>
-      <c r="G49" s="29"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>44</v>
+        <v>276</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E50" s="30">
         <v>10</v>
@@ -2542,20 +2412,19 @@
       <c r="F50" s="34">
         <v>0</v>
       </c>
-      <c r="G50" s="30"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>45</v>
+        <v>277</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E51" s="30">
         <v>10</v>
@@ -2563,20 +2432,19 @@
       <c r="F51" s="34">
         <v>0</v>
       </c>
-      <c r="G51" s="30"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>46</v>
+        <v>277</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E52" s="30">
         <v>10</v>
@@ -2584,20 +2452,19 @@
       <c r="F52" s="34">
         <v>0</v>
       </c>
-      <c r="G52" s="30"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>51</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E53" s="30">
         <v>10</v>
@@ -2605,22 +2472,19 @@
       <c r="F53" s="34">
         <v>46</v>
       </c>
-      <c r="G53" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>48</v>
+        <v>276</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E54" s="30">
         <v>10</v>
@@ -2628,28 +2492,26 @@
       <c r="F54" s="34">
         <v>0</v>
       </c>
-      <c r="G54" s="30"/>
-    </row>
-    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>53</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="E55" s="30">
         <v>11</v>
       </c>
       <c r="F55" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="G55" s="30"/>
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2661,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A12D3C-F185-4C2F-BC8E-E636E865D27E}">
   <dimension ref="A2:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2676,22 +2538,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2699,10 +2561,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>37</v>
@@ -2717,10 +2579,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>35</v>
@@ -2735,10 +2597,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D5" s="38" t="s">
         <v>22</v>
@@ -2747,7 +2609,7 @@
         <v>54</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2755,10 +2617,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>30</v>
@@ -2773,10 +2635,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>37</v>
@@ -2791,10 +2653,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>30</v>
@@ -2809,13 +2671,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E9" s="39">
         <v>54</v>
@@ -2827,19 +2689,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E10" s="39">
         <v>54</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2847,13 +2709,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E11" s="39">
         <v>54</v>
@@ -2865,19 +2727,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E12" s="39">
         <v>54</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,13 +2747,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E13" s="39">
         <v>54</v>
@@ -2903,13 +2765,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E14" s="39">
         <v>54</v>
@@ -2921,10 +2783,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>22</v>
@@ -2939,10 +2801,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>37</v>
@@ -2957,10 +2819,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>37</v>
@@ -2975,10 +2837,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>22</v>
@@ -2993,10 +2855,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="39">
@@ -3009,13 +2871,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E20" s="39">
         <v>54</v>
@@ -3027,13 +2889,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E21" s="39">
         <v>54</v>
@@ -3045,13 +2907,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E22" s="39">
         <v>54</v>
@@ -3063,10 +2925,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>17</v>
@@ -3081,19 +2943,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E24" s="39">
         <v>54</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3101,13 +2963,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E25" s="39">
         <v>54</v>
@@ -3119,13 +2981,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E26" s="39">
         <v>54</v>
@@ -3137,10 +2999,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>37</v>
@@ -3155,13 +3017,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E28" s="39">
         <v>54</v>
@@ -3173,13 +3035,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E29" s="39">
         <v>54</v>
@@ -3191,10 +3053,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>30</v>
@@ -3209,10 +3071,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>22</v>
@@ -3227,13 +3089,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E32" s="39">
         <v>54</v>
@@ -3245,10 +3107,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>37</v>
@@ -3257,7 +3119,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="40" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3265,13 +3127,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="E34" s="39">
         <v>54</v>
@@ -3283,10 +3145,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>30</v>
@@ -3301,10 +3163,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>30</v>
@@ -3319,13 +3181,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E37" s="39">
         <v>54</v>
@@ -3337,13 +3199,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E38" s="39">
         <v>54</v>
@@ -3355,13 +3217,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="E39" s="39">
         <v>54</v>
@@ -3373,10 +3235,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>36</v>
@@ -3391,13 +3253,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="E41" s="39">
         <v>54</v>
@@ -3409,10 +3271,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>31</v>
@@ -3427,10 +3289,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D43" s="38" t="s">
         <v>37</v>
@@ -3445,10 +3307,10 @@
         <v>2</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D44" s="38" t="s">
         <v>31</v>
@@ -3463,10 +3325,10 @@
         <v>2</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>36</v>
@@ -3481,13 +3343,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="E46" s="39">
         <v>54</v>
@@ -3499,13 +3361,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E47" s="39">
         <v>54</v>
@@ -3517,10 +3379,10 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>31</v>
@@ -3535,13 +3397,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="E49" s="39">
         <v>54</v>
@@ -3553,13 +3415,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E50" s="39">
         <v>54</v>
@@ -3571,10 +3433,10 @@
         <v>2</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>36</v>
@@ -3589,10 +3451,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>22</v>
@@ -3607,10 +3469,10 @@
         <v>2</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>33</v>
@@ -3625,10 +3487,10 @@
         <v>2</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>31</v>
@@ -3637,7 +3499,7 @@
         <v>54</v>
       </c>
       <c r="F54" s="40" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3645,13 +3507,13 @@
         <v>2</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="E55" s="39">
         <v>54</v>
@@ -3665,10 +3527,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218295B3-95C6-4056-8916-38091AF1344F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,90 +3542,218 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>280</v>
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>281</v>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>280</v>
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>282</v>
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>285</v>
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>286</v>
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>286</v>
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>287</v>
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>288</v>
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>94</v>
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alfa casi lista, se arreglo la equivalencia de ramos con sus pesos correcto y de los electivos (revisado con 2018)
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F8651-4962-4509-8A0F-79E7936F6F77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D01E0-2DF8-46C5-B739-3A55C4881B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="13890" yWindow="1395" windowWidth="18000" windowHeight="9810" firstSheet="1" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="278">
   <si>
     <t>CBM1000</t>
   </si>
@@ -627,9 +627,6 @@
     <t>CIT3335</t>
   </si>
   <si>
-    <t>INTERFACE HUMANE MÁQUINA</t>
-  </si>
-  <si>
     <t>CIT2005, CIT2104</t>
   </si>
   <si>
@@ -871,6 +868,9 @@
   </si>
   <si>
     <t>CIT34XX</t>
+  </si>
+  <si>
+    <t>INTERFACE HUMANO MÁQUINA</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1001,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1039,12 +1039,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1089,9 +1109,15 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1119,7 +1145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1417,11 +1443,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1860,7 +1886,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1980,7 +2006,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>107</v>
@@ -2201,7 +2227,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>107</v>
@@ -2298,7 +2324,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>38</v>
@@ -2318,7 +2344,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>38</v>
@@ -2338,7 +2364,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>38</v>
@@ -2378,7 +2404,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>38</v>
@@ -2398,7 +2424,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>38</v>
@@ -2418,7 +2444,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>38</v>
@@ -2438,7 +2464,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>38</v>
@@ -2478,7 +2504,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>38</v>
@@ -2504,7 +2530,7 @@
         <v>106</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E55" s="30">
         <v>11</v>
@@ -2523,11 +2549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A12D3C-F185-4C2F-BC8E-E636E865D27E}">
   <dimension ref="A2:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
@@ -2984,10 +3010,10 @@
         <v>195</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D26" s="38" t="s">
         <v>196</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>197</v>
       </c>
       <c r="E26" s="39">
         <v>54</v>
@@ -2999,10 +3025,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>37</v>
@@ -3017,13 +3043,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="38" t="s">
         <v>201</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>202</v>
       </c>
       <c r="E28" s="39">
         <v>54</v>
@@ -3035,13 +3061,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="38" t="s">
         <v>204</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>205</v>
       </c>
       <c r="E29" s="39">
         <v>54</v>
@@ -3053,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>30</v>
@@ -3071,10 +3097,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>22</v>
@@ -3089,13 +3115,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>211</v>
-      </c>
       <c r="D32" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E32" s="39">
         <v>54</v>
@@ -3107,10 +3133,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>37</v>
@@ -3119,7 +3145,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3127,13 +3153,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="38" t="s">
         <v>216</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>217</v>
       </c>
       <c r="E34" s="39">
         <v>54</v>
@@ -3145,10 +3171,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>30</v>
@@ -3163,10 +3189,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>30</v>
@@ -3181,13 +3207,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="38" t="s">
         <v>223</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>224</v>
       </c>
       <c r="E37" s="39">
         <v>54</v>
@@ -3199,13 +3225,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="38" t="s">
         <v>226</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>227</v>
       </c>
       <c r="E38" s="39">
         <v>54</v>
@@ -3217,13 +3243,13 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="38" t="s">
         <v>229</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>230</v>
       </c>
       <c r="E39" s="39">
         <v>54</v>
@@ -3235,10 +3261,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>36</v>
@@ -3253,13 +3279,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="D41" s="38" t="s">
         <v>234</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>235</v>
       </c>
       <c r="E41" s="39">
         <v>54</v>
@@ -3271,10 +3297,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>31</v>
@@ -3289,10 +3315,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="D43" s="38" t="s">
         <v>37</v>
@@ -3307,10 +3333,10 @@
         <v>2</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="D44" s="38" t="s">
         <v>31</v>
@@ -3325,10 +3351,10 @@
         <v>2</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>243</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>36</v>
@@ -3343,13 +3369,13 @@
         <v>2</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>245</v>
-      </c>
       <c r="D46" s="38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E46" s="39">
         <v>54</v>
@@ -3361,13 +3387,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>247</v>
-      </c>
       <c r="D47" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E47" s="39">
         <v>54</v>
@@ -3379,10 +3405,10 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>31</v>
@@ -3397,13 +3423,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="38" t="s">
         <v>251</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>252</v>
       </c>
       <c r="E49" s="39">
         <v>54</v>
@@ -3415,13 +3441,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="38" t="s">
         <v>254</v>
-      </c>
-      <c r="D50" s="38" t="s">
-        <v>255</v>
       </c>
       <c r="E50" s="39">
         <v>54</v>
@@ -3433,10 +3459,10 @@
         <v>2</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>36</v>
@@ -3451,10 +3477,10 @@
         <v>2</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>22</v>
@@ -3469,10 +3495,10 @@
         <v>2</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>33</v>
@@ -3487,10 +3513,10 @@
         <v>2</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>31</v>
@@ -3499,7 +3525,7 @@
         <v>54</v>
       </c>
       <c r="F54" s="40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3507,13 +3533,13 @@
         <v>2</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="D55" s="38" t="s">
         <v>266</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>267</v>
       </c>
       <c r="E55" s="39">
         <v>54</v>
@@ -3527,13 +3553,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218295B3-95C6-4056-8916-38091AF1344F}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>
@@ -3542,10 +3568,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>268</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3609,7 +3635,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3620,7 +3646,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -3630,130 +3656,138 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>113</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>273</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>121</v>
+        <v>25</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>126</v>
+      <c r="A27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se fija como maximo 6 recomendaciones de secciones por semestre y se borran las secciones de menor peso
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D01E0-2DF8-46C5-B739-3A55C4881B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72203D63-B504-45F0-BF90-1F8FE2FE1A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="1395" windowWidth="18000" windowHeight="9810" firstSheet="1" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="10140" yWindow="3570" windowWidth="18000" windowHeight="9810" activeTab="1" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="276">
   <si>
     <t>CBM1000</t>
   </si>
@@ -565,12 +565,6 @@
   </si>
   <si>
     <t>ESTRATEGIAS DE PROGRAMACIÓN</t>
-  </si>
-  <si>
-    <t>CIT3334</t>
-  </si>
-  <si>
-    <t>ESTRUCTURAS DE DATOS COMPACTAS</t>
   </si>
   <si>
     <t>CIT3328</t>
@@ -1443,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,7 +1880,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -2006,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>107</v>
@@ -2227,7 +2221,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>107</v>
@@ -2324,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>38</v>
@@ -2344,7 +2338,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>38</v>
@@ -2364,7 +2358,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>38</v>
@@ -2404,7 +2398,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>38</v>
@@ -2424,7 +2418,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>38</v>
@@ -2444,7 +2438,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>38</v>
@@ -2464,7 +2458,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>38</v>
@@ -2504,7 +2498,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>38</v>
@@ -2530,7 +2524,7 @@
         <v>106</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E55" s="30">
         <v>11</v>
@@ -2547,18 +2541,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A12D3C-F185-4C2F-BC8E-E636E865D27E}">
-  <dimension ref="A2:F55"/>
+  <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2573,10 +2567,10 @@
         <v>134</v>
       </c>
       <c r="D2" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>135</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>136</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>137</v>
@@ -2592,11 +2586,11 @@
       <c r="C3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39">
+        <v>54</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="39">
-        <v>54</v>
       </c>
       <c r="F3" s="40"/>
     </row>
@@ -2610,11 +2604,11 @@
       <c r="C4" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="39">
+        <v>54</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>35</v>
-      </c>
-      <c r="E4" s="39">
-        <v>54</v>
       </c>
       <c r="F4" s="40"/>
     </row>
@@ -2628,11 +2622,11 @@
       <c r="C5" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="39">
+        <v>54</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="39">
-        <v>54</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>144</v>
@@ -2648,11 +2642,11 @@
       <c r="C6" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="39">
+        <v>54</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="39">
-        <v>54</v>
       </c>
       <c r="F6" s="40"/>
     </row>
@@ -2666,11 +2660,11 @@
       <c r="C7" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="39">
+        <v>54</v>
+      </c>
+      <c r="E7" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" s="39">
-        <v>54</v>
       </c>
       <c r="F7" s="40"/>
     </row>
@@ -2684,11 +2678,11 @@
       <c r="C8" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="39">
+        <v>54</v>
+      </c>
+      <c r="E8" s="38" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="39">
-        <v>54</v>
       </c>
       <c r="F8" s="40"/>
     </row>
@@ -2702,11 +2696,11 @@
       <c r="C9" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="39">
+        <v>54</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>153</v>
-      </c>
-      <c r="E9" s="39">
-        <v>54</v>
       </c>
       <c r="F9" s="40"/>
     </row>
@@ -2720,11 +2714,11 @@
       <c r="C10" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="39">
+        <v>54</v>
+      </c>
+      <c r="E10" s="38" t="s">
         <v>156</v>
-      </c>
-      <c r="E10" s="39">
-        <v>54</v>
       </c>
       <c r="F10" s="40" t="s">
         <v>123</v>
@@ -2740,11 +2734,11 @@
       <c r="C11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="39">
+        <v>54</v>
+      </c>
+      <c r="E11" s="38" t="s">
         <v>156</v>
-      </c>
-      <c r="E11" s="39">
-        <v>54</v>
       </c>
       <c r="F11" s="40"/>
     </row>
@@ -2758,11 +2752,11 @@
       <c r="C12" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39">
+        <v>54</v>
+      </c>
+      <c r="E12" s="38" t="s">
         <v>161</v>
-      </c>
-      <c r="E12" s="39">
-        <v>54</v>
       </c>
       <c r="F12" s="40" t="s">
         <v>123</v>
@@ -2778,11 +2772,11 @@
       <c r="C13" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="39">
+        <v>54</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>164</v>
-      </c>
-      <c r="E13" s="39">
-        <v>54</v>
       </c>
       <c r="F13" s="40"/>
     </row>
@@ -2796,11 +2790,11 @@
       <c r="C14" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="39">
+        <v>54</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>167</v>
-      </c>
-      <c r="E14" s="39">
-        <v>54</v>
       </c>
       <c r="F14" s="40"/>
     </row>
@@ -2814,11 +2808,11 @@
       <c r="C15" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="39">
+        <v>54</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>22</v>
-      </c>
-      <c r="E15" s="39">
-        <v>54</v>
       </c>
       <c r="F15" s="40"/>
     </row>
@@ -2832,11 +2826,11 @@
       <c r="C16" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="39">
+        <v>54</v>
+      </c>
+      <c r="E16" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="E16" s="39">
-        <v>54</v>
       </c>
       <c r="F16" s="40"/>
     </row>
@@ -2850,11 +2844,11 @@
       <c r="C17" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="39">
+        <v>54</v>
+      </c>
+      <c r="E17" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="E17" s="39">
-        <v>54</v>
       </c>
       <c r="F17" s="40"/>
     </row>
@@ -2868,11 +2862,11 @@
       <c r="C18" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="39">
+        <v>54</v>
+      </c>
+      <c r="E18" s="38" t="s">
         <v>22</v>
-      </c>
-      <c r="E18" s="39">
-        <v>54</v>
       </c>
       <c r="F18" s="40"/>
     </row>
@@ -2886,9 +2880,11 @@
       <c r="C19" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39">
-        <v>54</v>
+      <c r="D19" s="39">
+        <v>54</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>178</v>
       </c>
       <c r="F19" s="40"/>
     </row>
@@ -2897,16 +2893,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="39">
+        <v>54</v>
+      </c>
+      <c r="E20" s="38" t="s">
         <v>178</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20" s="39">
-        <v>54</v>
       </c>
       <c r="F20" s="40"/>
     </row>
@@ -2920,11 +2916,11 @@
       <c r="C21" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="E21" s="39">
-        <v>54</v>
+      <c r="D21" s="39">
+        <v>54</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>183</v>
       </c>
       <c r="F21" s="40"/>
     </row>
@@ -2933,16 +2929,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D22" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="39">
-        <v>54</v>
+      <c r="D22" s="39">
+        <v>54</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -2956,49 +2952,49 @@
       <c r="C23" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="39">
-        <v>54</v>
-      </c>
-      <c r="F23" s="40"/>
+      <c r="D23" s="39">
+        <v>54</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>1</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="E24" s="39">
-        <v>54</v>
-      </c>
-      <c r="F24" s="40" t="s">
         <v>191</v>
       </c>
+      <c r="D24" s="39">
+        <v>54</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="40"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D25" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="39">
+        <v>54</v>
+      </c>
+      <c r="E25" s="38" t="s">
         <v>194</v>
-      </c>
-      <c r="E25" s="39">
-        <v>54</v>
       </c>
       <c r="F25" s="40"/>
     </row>
@@ -3010,13 +3006,13 @@
         <v>195</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D26" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="E26" s="39">
-        <v>54</v>
+      <c r="D26" s="39">
+        <v>54</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="F26" s="40"/>
     </row>
@@ -3030,11 +3026,11 @@
       <c r="C27" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D27" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="39">
-        <v>54</v>
+      <c r="D27" s="39">
+        <v>54</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>199</v>
       </c>
       <c r="F27" s="40"/>
     </row>
@@ -3043,16 +3039,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="E28" s="39">
-        <v>54</v>
+      <c r="D28" s="39">
+        <v>54</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>202</v>
       </c>
       <c r="F28" s="40"/>
     </row>
@@ -3061,16 +3057,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="39">
-        <v>54</v>
+      <c r="D29" s="39">
+        <v>54</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="F29" s="40"/>
     </row>
@@ -3084,11 +3080,11 @@
       <c r="C30" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D30" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="39">
-        <v>54</v>
+      <c r="D30" s="39">
+        <v>54</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="F30" s="40"/>
     </row>
@@ -3102,11 +3098,11 @@
       <c r="C31" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D31" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="39">
-        <v>54</v>
+      <c r="D31" s="39">
+        <v>54</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>199</v>
       </c>
       <c r="F31" s="40"/>
     </row>
@@ -3120,49 +3116,49 @@
       <c r="C32" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D32" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="E32" s="39">
-        <v>54</v>
-      </c>
-      <c r="F32" s="40"/>
+      <c r="D32" s="39">
+        <v>54</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="39">
-        <v>54</v>
-      </c>
-      <c r="F33" s="40" t="s">
         <v>213</v>
       </c>
+      <c r="D33" s="39">
+        <v>54</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D34" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E34" s="39">
-        <v>54</v>
+      <c r="D34" s="39">
+        <v>54</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="F34" s="40"/>
     </row>
@@ -3176,11 +3172,11 @@
       <c r="C35" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="39">
+        <v>54</v>
+      </c>
+      <c r="E35" s="38" t="s">
         <v>30</v>
-      </c>
-      <c r="E35" s="39">
-        <v>54</v>
       </c>
       <c r="F35" s="40"/>
     </row>
@@ -3194,29 +3190,29 @@
       <c r="C36" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D36" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="39">
-        <v>54</v>
+      <c r="D36" s="39">
+        <v>54</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>221</v>
       </c>
       <c r="F36" s="40"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E37" s="39">
-        <v>54</v>
+      <c r="D37" s="39">
+        <v>54</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="F37" s="40"/>
     </row>
@@ -3225,16 +3221,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D38" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="39">
-        <v>54</v>
+      <c r="D38" s="39">
+        <v>54</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>227</v>
       </c>
       <c r="F38" s="40"/>
     </row>
@@ -3243,16 +3239,16 @@
         <v>2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D39" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="E39" s="39">
-        <v>54</v>
+      <c r="D39" s="39">
+        <v>54</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>36</v>
       </c>
       <c r="F39" s="40"/>
     </row>
@@ -3266,11 +3262,11 @@
       <c r="C40" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="D40" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="39">
-        <v>54</v>
+      <c r="D40" s="39">
+        <v>54</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>232</v>
       </c>
       <c r="F40" s="40"/>
     </row>
@@ -3279,16 +3275,16 @@
         <v>2</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D41" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="E41" s="39">
-        <v>54</v>
+      <c r="D41" s="39">
+        <v>54</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="F41" s="40"/>
     </row>
@@ -3302,11 +3298,11 @@
       <c r="C42" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D42" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="39">
-        <v>54</v>
+      <c r="D42" s="39">
+        <v>54</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="F42" s="40"/>
     </row>
@@ -3320,11 +3316,11 @@
       <c r="C43" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="D43" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="39">
-        <v>54</v>
+      <c r="D43" s="39">
+        <v>54</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="F43" s="40"/>
     </row>
@@ -3338,11 +3334,11 @@
       <c r="C44" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="D44" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" s="39">
-        <v>54</v>
+      <c r="D44" s="39">
+        <v>54</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>36</v>
       </c>
       <c r="F44" s="40"/>
     </row>
@@ -3356,11 +3352,11 @@
       <c r="C45" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D45" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="39">
-        <v>54</v>
+      <c r="D45" s="39">
+        <v>54</v>
+      </c>
+      <c r="E45" s="38" t="s">
+        <v>227</v>
       </c>
       <c r="F45" s="40"/>
     </row>
@@ -3374,11 +3370,11 @@
       <c r="C46" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="D46" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" s="39">
-        <v>54</v>
+      <c r="D46" s="39">
+        <v>54</v>
+      </c>
+      <c r="E46" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="F46" s="40"/>
     </row>
@@ -3392,11 +3388,11 @@
       <c r="C47" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D47" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="E47" s="39">
-        <v>54</v>
+      <c r="D47" s="39">
+        <v>54</v>
+      </c>
+      <c r="E47" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="F47" s="40"/>
     </row>
@@ -3410,11 +3406,11 @@
       <c r="C48" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="D48" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" s="39">
-        <v>54</v>
+      <c r="D48" s="39">
+        <v>54</v>
+      </c>
+      <c r="E48" s="38" t="s">
+        <v>249</v>
       </c>
       <c r="F48" s="40"/>
     </row>
@@ -3423,16 +3419,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="D49" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="E49" s="39">
-        <v>54</v>
+      <c r="D49" s="39">
+        <v>54</v>
+      </c>
+      <c r="E49" s="38" t="s">
+        <v>252</v>
       </c>
       <c r="F49" s="40"/>
     </row>
@@ -3441,16 +3437,16 @@
         <v>2</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D50" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="E50" s="39">
-        <v>54</v>
+      <c r="D50" s="39">
+        <v>54</v>
+      </c>
+      <c r="E50" s="38" t="s">
+        <v>36</v>
       </c>
       <c r="F50" s="40"/>
     </row>
@@ -3464,11 +3460,11 @@
       <c r="C51" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D51" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="39">
-        <v>54</v>
+      <c r="D51" s="39">
+        <v>54</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="F51" s="40"/>
     </row>
@@ -3482,11 +3478,11 @@
       <c r="C52" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D52" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" s="39">
-        <v>54</v>
+      <c r="D52" s="39">
+        <v>54</v>
+      </c>
+      <c r="E52" s="38" t="s">
+        <v>33</v>
       </c>
       <c r="F52" s="40"/>
     </row>
@@ -3500,51 +3496,33 @@
       <c r="C53" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="D53" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="39">
-        <v>54</v>
-      </c>
-      <c r="F53" s="40"/>
+      <c r="D53" s="39">
+        <v>54</v>
+      </c>
+      <c r="E53" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>2</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D54" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" s="39">
-        <v>54</v>
-      </c>
-      <c r="F54" s="40" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="10">
-        <v>2</v>
-      </c>
-      <c r="B55" s="7" t="s">
+      <c r="D54" s="39">
+        <v>54</v>
+      </c>
+      <c r="E54" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="E55" s="39">
-        <v>54</v>
-      </c>
-      <c r="F55" s="40"/>
+      <c r="F54" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3568,10 +3546,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3635,7 +3613,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3659,7 +3637,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3776,7 +3754,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B27" s="42" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
falta modificar el archivo extract_data ya que se borraron los cambios
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC3A4F-524B-4F48-A4FF-787F53F69D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11050D84-6062-4F44-BFE2-A4B734793258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="1935" windowWidth="20730" windowHeight="11760" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
api google to login and register
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E43D4B-27A4-442D-BC6C-A9331C1AB1B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4A18FB-F369-4010-8714-9F30D73C20A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,7 +3533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218295B3-95C6-4056-8916-38091AF1344F}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
alfa 4.0, falta mostrar mas opciones y ver las vacantes de las secciones
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11050D84-6062-4F44-BFE2-A4B734793258}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCBB67A-45A2-413B-B27B-E1C54E34A5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -865,75 +865,74 @@
     <t>CIT5002</t>
   </si>
   <si>
-    <t>3, 10, 13 , 17, 20, 26, 27, 28, 29,
- 36, 37, 38, 39, 40, 42, 43, 44, 
+    <t>CFG-1</t>
+  </si>
+  <si>
+    <t>CFG-2</t>
+  </si>
+  <si>
+    <t>CFG-3</t>
+  </si>
+  <si>
+    <t>CFG-4</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 1</t>
+  </si>
+  <si>
+    <t>CIT3310</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 2</t>
+  </si>
+  <si>
+    <t>CIT3311</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 4</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 3</t>
+  </si>
+  <si>
+    <t>CIT3312</t>
+  </si>
+  <si>
+    <t>CIT3313</t>
+  </si>
+  <si>
+    <t>CIT3410</t>
+  </si>
+  <si>
+    <t>CIT3411</t>
+  </si>
+  <si>
+    <t>CIT3412</t>
+  </si>
+  <si>
+    <t>CIT3413</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 4</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 3</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 2</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 1</t>
+  </si>
+  <si>
+    <t>53, 26, 27, 28, 29, 33, 36, 37, 38, 39 ,40 , 41, 42</t>
+  </si>
+  <si>
+    <t>3,10, 13, 15, 16, 17, 18 ,19 ,20, 21</t>
+  </si>
+  <si>
+    <t>43, 44, 
 45, 47, 48, 49, 50, 51, 52,53,54</t>
-  </si>
-  <si>
-    <t>CFG-1</t>
-  </si>
-  <si>
-    <t>CFG-2</t>
-  </si>
-  <si>
-    <t>CFG-3</t>
-  </si>
-  <si>
-    <t>CFG-4</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 1</t>
-  </si>
-  <si>
-    <t>CIT3310</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 2</t>
-  </si>
-  <si>
-    <t>CIT3311</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 4</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 3</t>
-  </si>
-  <si>
-    <t>CIT3312</t>
-  </si>
-  <si>
-    <t>CIT3313</t>
-  </si>
-  <si>
-    <t>CIT3410</t>
-  </si>
-  <si>
-    <t>CIT3411</t>
-  </si>
-  <si>
-    <t>CIT3412</t>
-  </si>
-  <si>
-    <t>CIT3413</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 4</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 3</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 2</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 1</t>
-  </si>
-  <si>
-    <t>53, 26, 27, 28, 29, 33, 36, 37, 38, 39 ,40 , 41, 42</t>
-  </si>
-  <si>
-    <t>3,10, 13, 15, 16, 17, 18 ,19 ,20, 21</t>
   </si>
 </sst>
 </file>
@@ -1554,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,10 +1773,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="46">
         <v>0</v>
@@ -1974,10 +1973,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D21" s="48">
         <v>0</v>
@@ -2094,10 +2093,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D27" s="49">
         <v>0</v>
@@ -2415,10 +2414,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D43" s="53">
         <v>0</v>
@@ -2435,10 +2434,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D44" s="54">
         <v>0</v>
@@ -2455,10 +2454,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D45" s="54">
         <v>0</v>
@@ -2475,10 +2474,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D46" s="54">
         <v>0</v>
@@ -2515,10 +2514,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D48" s="54">
         <v>0</v>
@@ -2535,10 +2534,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D49" s="36">
         <v>0</v>
@@ -2555,10 +2554,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D50" s="36">
         <v>0</v>
@@ -2575,10 +2574,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="D51" s="36">
         <v>0</v>
@@ -2615,10 +2614,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D53" s="36">
         <v>0</v>
@@ -2641,7 +2640,7 @@
         <v>271</v>
       </c>
       <c r="D54" s="57" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E54" s="58" t="s">
         <v>105</v>
@@ -2659,14 +2658,14 @@
         <v>274</v>
       </c>
       <c r="D55" s="57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E55" s="58" t="s">
         <v>105</v>
       </c>
       <c r="F55" s="59"/>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>99</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>104</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>264</v>

</xml_diff>

<commit_message>
alfa lista con revisando las vacantes de las secciones
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCBB67A-45A2-413B-B27B-E1C54E34A5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E40726-93CA-46F7-B2A3-6267FF02A448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -1553,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
@@ -3685,8 +3685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218295B3-95C6-4056-8916-38091AF1344F}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,5 +3922,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add initial front and function to get sections avaibles of a user and little change in clique
</commit_message>
<xml_diff>
--- a/RutaCritica/MallaCurricular2010.xlsx
+++ b/RutaCritica/MallaCurricular2010.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79055EF3-2AA2-48CA-8CB9-F5B8B3EC593F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1620AA-3D24-4DD1-ACAD-FC1EA98F5A9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="MallaCurricular2010" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="299">
   <si>
     <t>CBM1000</t>
   </si>
@@ -933,18 +933,6 @@
   <si>
     <t>43, 44, 
 45, 47, 48, 49, 50, 51, 52,53,54</t>
-  </si>
-  <si>
-    <t>CFG3</t>
-  </si>
-  <si>
-    <t>CFG2</t>
-  </si>
-  <si>
-    <t>CFG1</t>
-  </si>
-  <si>
-    <t>CFG4</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1227,7 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1267,7 +1255,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1566,10 +1554,10 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1785,7 +1773,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>276</v>
@@ -1985,7 +1973,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>277</v>
@@ -2105,7 +2093,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>278</v>
@@ -2426,7 +2414,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>279</v>
@@ -2711,7 +2699,7 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
@@ -3701,7 +3689,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" customWidth="1"/>

</xml_diff>